<commit_message>
assetbuild now creates nonexistent directories; new gamemode system
</commit_message>
<xml_diff>
--- a/q2-bringup.xlsx
+++ b/q2-bringup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99F68A70-9A7F-41D3-A040-D1D632C4B7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C38A250-E0F3-4FD0-9044-105200551046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>gamex64</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Cleaned up audio</t>
+  </si>
+  <si>
+    <t>"""Asset Pipeline""" / TGA part 1</t>
+  </si>
+  <si>
+    <t>Some asset removals, obsolete GL code removal (gl_3dlabs_broken)</t>
+  </si>
+  <si>
+    <t>Remove mono lightmaps</t>
+  </si>
+  <si>
+    <t>Remove 3dfx, 3DLabs, 1st gen PowerVR specific code</t>
+  </si>
+  <si>
+    <t>TGA part 2, 256-color nuking (although skins don't work yet)</t>
   </si>
 </sst>
 </file>
@@ -441,7 +456,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F18" sqref="A1:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +515,7 @@
         <v>411136</v>
       </c>
       <c r="E2">
-        <f>SUM(B2:D2)</f>
+        <f t="shared" ref="E2:E24" si="0">SUM(B2:D2)</f>
         <v>3037184</v>
       </c>
       <c r="F2">
@@ -532,7 +547,7 @@
         <v>411136</v>
       </c>
       <c r="E3">
-        <f>SUM(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>3037184</v>
       </c>
       <c r="F3">
@@ -564,7 +579,7 @@
         <v>411136</v>
       </c>
       <c r="E4">
-        <f>SUM(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>3037184</v>
       </c>
       <c r="F4">
@@ -596,7 +611,7 @@
         <v>411136</v>
       </c>
       <c r="E5">
-        <f>SUM(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>3023872</v>
       </c>
       <c r="F5">
@@ -628,7 +643,7 @@
         <v>411136</v>
       </c>
       <c r="E6">
-        <f>SUM(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>3011584</v>
       </c>
       <c r="F6">
@@ -660,7 +675,7 @@
         <v>411136</v>
       </c>
       <c r="E7">
-        <f>SUM(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>3005952</v>
       </c>
       <c r="F7">
@@ -692,7 +707,7 @@
         <v>411136</v>
       </c>
       <c r="E8">
-        <f>SUM(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>3137024</v>
       </c>
       <c r="F8">
@@ -724,7 +739,7 @@
         <v>411136</v>
       </c>
       <c r="E9">
-        <f>SUM(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>3137024</v>
       </c>
       <c r="F9">
@@ -756,7 +771,7 @@
         <v>411136</v>
       </c>
       <c r="E10">
-        <f>SUM(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>2915328</v>
       </c>
       <c r="F10">
@@ -788,7 +803,7 @@
         <v>411136</v>
       </c>
       <c r="E11">
-        <f>SUM(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>2908160</v>
       </c>
       <c r="F11">
@@ -820,7 +835,7 @@
         <v>411136</v>
       </c>
       <c r="E12">
-        <f>SUM(B12:D12)</f>
+        <f t="shared" si="0"/>
         <v>2908160</v>
       </c>
       <c r="F12">
@@ -839,78 +854,168 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45253.962500000001</v>
+      </c>
+      <c r="B13">
+        <v>1789952</v>
+      </c>
+      <c r="C13">
+        <v>704000</v>
+      </c>
+      <c r="D13">
+        <v>411136</v>
+      </c>
       <c r="E13">
-        <f>SUM(B13:D13)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2905088</v>
+      </c>
+      <c r="F13">
+        <v>96018618</v>
       </c>
       <c r="G13" s="2">
         <f>1-(E13/E2)</f>
-        <v>1</v>
+        <v>4.3492919757248782E-2</v>
       </c>
       <c r="H13" s="2">
         <f>1-(F13/F2)</f>
-        <v>1</v>
+        <v>0.79693314126876946</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45253.990277777775</v>
+      </c>
+      <c r="B14">
+        <v>1789440</v>
+      </c>
+      <c r="C14">
+        <v>704000</v>
+      </c>
+      <c r="D14">
+        <v>407552</v>
+      </c>
       <c r="E14">
-        <f>SUM(B14:D14)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2900992</v>
+      </c>
+      <c r="F14">
+        <v>95932487</v>
       </c>
       <c r="G14" s="2">
         <f>1-(E14/E2)</f>
-        <v>1</v>
+        <v>4.484153742414021E-2</v>
       </c>
       <c r="H14" s="2">
         <f>1-(F14/F2)</f>
-        <v>1</v>
+        <v>0.79711529710451967</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45253.99722222222</v>
+      </c>
+      <c r="B15">
+        <v>1789440</v>
+      </c>
+      <c r="C15">
+        <v>704000</v>
+      </c>
+      <c r="D15">
+        <v>404480</v>
+      </c>
       <c r="E15">
-        <f>SUM(B15:D15)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2897920</v>
+      </c>
+      <c r="F15">
+        <v>98426571</v>
       </c>
       <c r="G15" s="2">
         <f>1-(E15/E2)</f>
-        <v>1</v>
+        <v>4.5853000674308864E-2</v>
       </c>
       <c r="H15" s="2">
         <f>1-(F15/F2)</f>
-        <v>1</v>
+        <v>0.79184063460842102</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45254.001388888886</v>
+      </c>
+      <c r="B16">
+        <v>1789440</v>
+      </c>
+      <c r="C16">
+        <v>704000</v>
+      </c>
+      <c r="D16">
+        <v>403456</v>
+      </c>
       <c r="E16">
-        <f>SUM(B16:D16)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2896896</v>
+      </c>
+      <c r="F16">
+        <v>98426571</v>
       </c>
       <c r="G16" s="2">
         <f>1-(E16/E2)</f>
-        <v>1</v>
+        <v>4.6190155091031637E-2</v>
       </c>
       <c r="H16" s="2">
         <f>1-(F16/F2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+        <v>0.79184063460842102</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45254.072916666664</v>
+      </c>
+      <c r="B17">
+        <v>1787392</v>
+      </c>
+      <c r="C17">
+        <v>704000</v>
+      </c>
+      <c r="D17">
+        <v>396288</v>
+      </c>
       <c r="E17">
-        <f>SUM(B17:D17)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2887680</v>
+      </c>
+      <c r="F17">
+        <v>168694067</v>
       </c>
       <c r="G17" s="2">
         <f>1-(E17/E2)</f>
-        <v>1</v>
+        <v>4.9224544841537377E-2</v>
       </c>
       <c r="H17" s="2">
         <f>1-(F17/F2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+        <v>0.64323404162840858</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E18">
-        <f>SUM(B18:D18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G18" s="2">
@@ -922,9 +1027,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E19">
-        <f>SUM(B19:D19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="2">
@@ -936,9 +1041,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20">
-        <f>SUM(B20:D20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G20" s="2">
@@ -950,9 +1055,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E21">
-        <f>SUM(B21:D21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G21" s="2">
@@ -964,9 +1069,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E22">
-        <f>SUM(B22:D22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" s="2">
@@ -978,9 +1083,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E23">
-        <f>SUM(B23:D23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" s="2">
@@ -992,9 +1097,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E24">
-        <f>SUM(B24:D24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" s="2">
@@ -1006,28 +1111,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fully remove PCX, rename deathmatch flags to game flags; remove null renderer; add some pipe textures and quit texture; update game config to remove palette
</commit_message>
<xml_diff>
--- a/q2-bringup.xlsx
+++ b/q2-bringup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C38A250-E0F3-4FD0-9044-105200551046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AC7648-4937-4F24-BB20-E69EDFC16AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>gamex64</t>
   </si>
@@ -100,6 +101,15 @@
   </si>
   <si>
     <t>TGA part 2, 256-color nuking (although skins don't work yet)</t>
+  </si>
+  <si>
+    <t>File reorg, gamemode system</t>
+  </si>
+  <si>
+    <t>Remove cinematics</t>
+  </si>
+  <si>
+    <t>Remove now-redundant menu options, remaining PCX support</t>
   </si>
 </sst>
 </file>
@@ -456,7 +466,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="A1:I24"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,45 +1024,99 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45256.945138888892</v>
+      </c>
+      <c r="B18">
+        <v>1786880</v>
+      </c>
+      <c r="C18">
+        <v>693248</v>
+      </c>
+      <c r="D18">
+        <v>396288</v>
+      </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2876416</v>
+      </c>
+      <c r="F18">
+        <v>168915701</v>
       </c>
       <c r="G18" s="2">
         <f>1-(E18/E2)</f>
-        <v>1</v>
+        <v>5.2933243425488885E-2</v>
       </c>
       <c r="H18" s="2">
         <f>1-(F18/F2)</f>
-        <v>1</v>
+        <v>0.64276531461373687</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45257.870833333334</v>
+      </c>
+      <c r="B19">
+        <v>1776640</v>
+      </c>
+      <c r="C19">
+        <v>693248</v>
+      </c>
+      <c r="D19">
+        <v>396288</v>
+      </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2866176</v>
+      </c>
+      <c r="F19">
+        <v>168970214</v>
       </c>
       <c r="G19" s="2">
         <f>1-(E19/E2)</f>
-        <v>1</v>
+        <v>5.6304787592717509E-2</v>
       </c>
       <c r="H19" s="2">
         <f>1-(F19/F2)</f>
-        <v>1</v>
+        <v>0.64265002672581895</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45257.890277777777</v>
+      </c>
+      <c r="B20">
+        <v>1776128</v>
+      </c>
+      <c r="C20">
+        <v>693248</v>
+      </c>
+      <c r="D20">
+        <v>392704</v>
+      </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2862080</v>
+      </c>
+      <c r="F20">
+        <v>168986319</v>
       </c>
       <c r="G20" s="2">
         <f>1-(E20/E2)</f>
-        <v>1</v>
+        <v>5.7653405259608936E-2</v>
       </c>
       <c r="H20" s="2">
         <f>1-(F20/F2)</f>
-        <v>1</v>
+        <v>0.64261596675049348</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
remove even more q2 code from gamex64. add zombies, absed on soldiers from q2 for now. more labrats tweaks
</commit_message>
<xml_diff>
--- a/q2-bringup.xlsx
+++ b/q2-bringup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AC7648-4937-4F24-BB20-E69EDFC16AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95A1F93E-EC18-47AA-9D08-E20A070516EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
+    <workbookView xWindow="13020" yWindow="1125" windowWidth="12975" windowHeight="12120" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>gamex64</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Remove now-redundant menu options, remaining PCX support</t>
+  </si>
+  <si>
+    <t>Remove software rendering menu and cvars</t>
+  </si>
+  <si>
+    <t>Remove duplicate TGA textures</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,31 +1126,67 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45258.681944444441</v>
+      </c>
+      <c r="B21">
+        <v>1776128</v>
+      </c>
+      <c r="C21">
+        <v>693760</v>
+      </c>
+      <c r="D21">
+        <v>392704</v>
+      </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2862592</v>
+      </c>
+      <c r="F21">
+        <v>170513693</v>
       </c>
       <c r="G21" s="2">
         <f>1-(E21/E2)</f>
-        <v>1</v>
+        <v>5.7484828051247439E-2</v>
       </c>
       <c r="H21" s="2">
         <f>1-(F21/F2)</f>
-        <v>1</v>
+        <v>0.63938576987047013</v>
+      </c>
+      <c r="I21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45258.779861111114</v>
+      </c>
+      <c r="B22">
+        <v>1776128</v>
+      </c>
+      <c r="C22">
+        <v>693760</v>
+      </c>
+      <c r="D22">
+        <v>392704</v>
+      </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2862592</v>
+      </c>
+      <c r="F22">
+        <v>151740398</v>
       </c>
       <c r="G22" s="2">
         <f>1-(E22/E2)</f>
-        <v>1</v>
+        <v>5.7484828051247439E-2</v>
       </c>
       <c r="H22" s="2">
         <f>1-(F22/F2)</f>
-        <v>1</v>
+        <v>0.67908884124444802</v>
+      </c>
+      <c r="I22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implement allowed teams functionality on items for zombie bamfuslicator, begin working on it
</commit_message>
<xml_diff>
--- a/q2-bringup.xlsx
+++ b/q2-bringup.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95A1F93E-EC18-47AA-9D08-E20A070516EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A308CA-065F-40C6-AE6B-017F59F97917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="1125" windowWidth="12975" windowHeight="12120" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>gamex64</t>
   </si>
@@ -116,6 +115,9 @@
   </si>
   <si>
     <t>Remove duplicate TGA textures</t>
+  </si>
+  <si>
+    <t>Remove all q2 enemies except infantry, add Zombie, remove all legacy OGL and more soft code, fix Draw_Fill usage</t>
   </si>
 </sst>
 </file>
@@ -472,7 +474,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +487,7 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="103.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1190,17 +1192,35 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45260.868055555555</v>
+      </c>
+      <c r="B23">
+        <v>1774592</v>
+      </c>
+      <c r="C23">
+        <v>612864</v>
+      </c>
+      <c r="D23">
+        <v>392192</v>
+      </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2779648</v>
+      </c>
+      <c r="F23">
+        <v>144108396</v>
       </c>
       <c r="G23" s="2">
         <f>1-(E23/E2)</f>
-        <v>1</v>
+        <v>8.4794335805799093E-2</v>
       </c>
       <c r="H23" s="2">
         <f>1-(F23/F2)</f>
-        <v>1</v>
+        <v>0.69522953045922575</v>
+      </c>
+      <c r="I23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
zombies disappear on being shot
</commit_message>
<xml_diff>
--- a/q2-bringup.xlsx
+++ b/q2-bringup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A308CA-065F-40C6-AE6B-017F59F97917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC67FE34-E036-4448-AF3B-306C28340B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>gamex64</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Remove all q2 enemies except infantry, add Zombie, remove all legacy OGL and more soft code, fix Draw_Fill usage</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 1</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,22 +1226,37 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <f>1-(E24/E2)</f>
-        <v>1</v>
-      </c>
-      <c r="H24" s="2">
-        <f>1-(F24/F2)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="2"/>
+      <c r="A25" s="1">
+        <v>45281.946527777778</v>
+      </c>
+      <c r="B25">
+        <v>1780736</v>
+      </c>
+      <c r="C25">
+        <v>600064</v>
+      </c>
+      <c r="D25">
+        <v>392192</v>
+      </c>
+      <c r="E25">
+        <f>SUM(B25:D25)</f>
+        <v>2772992</v>
+      </c>
+      <c r="F25">
+        <v>146996204</v>
+      </c>
+      <c r="G25" s="2">
+        <f>1-(E25/E2)</f>
+        <v>8.6985839514497676E-2</v>
+      </c>
+      <c r="H25" s="2">
+        <f>1-(F25/F2)</f>
+        <v>0.68912219303453059</v>
+      </c>
+      <c r="I25" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G26" s="2"/>

</xml_diff>

<commit_message>
remove buttons, just use images - might add them back
</commit_message>
<xml_diff>
--- a/q2-bringup.xlsx
+++ b/q2-bringup.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC67FE34-E036-4448-AF3B-306C28340B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B417427B-CBE3-4015-8EC3-47C5BBDE8D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Debug" sheetId="1" r:id="rId1"/>
+    <sheet name="Playtest or Release" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>gamex64</t>
   </si>
@@ -121,6 +122,24 @@
   </si>
   <si>
     <t>v0.0.4, prerelease 1</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 2</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 1 (early test)</t>
+  </si>
+  <si>
+    <t>Zombono</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 1 test</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 1 test4</t>
+  </si>
+  <si>
+    <t>Remove vulkan renderer</t>
   </si>
 </sst>
 </file>
@@ -477,7 +496,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +555,7 @@
         <v>411136</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">SUM(B2:D2)</f>
+        <f t="shared" ref="E2:E23" si="0">SUM(B2:D2)</f>
         <v>3037184</v>
       </c>
       <c r="F2">
@@ -1091,8 +1110,8 @@
         <v>5.6304787592717509E-2</v>
       </c>
       <c r="H19" s="2">
-        <f>1-(F19/F2)</f>
-        <v>0.64265002672581895</v>
+        <f>1-(F19/F3)</f>
+        <v>0.62517256497975404</v>
       </c>
       <c r="I19" t="s">
         <v>26</v>
@@ -1255,14 +1274,40 @@
         <v>0.68912219303453059</v>
       </c>
       <c r="I25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="2"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G27" s="2"/>
+      <c r="A27" s="1">
+        <v>45296.834027777775</v>
+      </c>
+      <c r="B27">
+        <v>1771520</v>
+      </c>
+      <c r="C27">
+        <v>603136</v>
+      </c>
+      <c r="D27">
+        <v>392704</v>
+      </c>
+      <c r="E27">
+        <f>SUM(B27:D27)</f>
+        <v>2767360</v>
+      </c>
+      <c r="F27">
+        <v>151311408</v>
+      </c>
+      <c r="G27" s="2">
+        <f>1-(E27/E4)</f>
+        <v>8.8840188806473375E-2</v>
+      </c>
+      <c r="H27" s="2">
+        <f>1-(F27/F4)</f>
+        <v>0.67113347551713654</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G28" s="2"/>
@@ -1298,4 +1343,205 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D702C5CE-747D-4EE4-B54A-F08904BF5F33}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45281.711111111108</v>
+      </c>
+      <c r="B2">
+        <v>930816</v>
+      </c>
+      <c r="C2">
+        <v>260608</v>
+      </c>
+      <c r="D2">
+        <v>147456</v>
+      </c>
+      <c r="E2">
+        <f>B2+C2+D2</f>
+        <v>1338880</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45281.845138888886</v>
+      </c>
+      <c r="B3">
+        <v>930304</v>
+      </c>
+      <c r="C3">
+        <v>260608</v>
+      </c>
+      <c r="D3">
+        <v>147456</v>
+      </c>
+      <c r="E3">
+        <f>B3+C3+D3</f>
+        <v>1338368</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45283.868055555555</v>
+      </c>
+      <c r="B4">
+        <v>927744</v>
+      </c>
+      <c r="C4">
+        <v>261120</v>
+      </c>
+      <c r="D4">
+        <v>147456</v>
+      </c>
+      <c r="E4">
+        <f>B4+C4+D4</f>
+        <v>1336320</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45291.893055555556</v>
+      </c>
+      <c r="B5">
+        <v>930816</v>
+      </c>
+      <c r="C5">
+        <v>262144</v>
+      </c>
+      <c r="D5">
+        <v>147456</v>
+      </c>
+      <c r="E5">
+        <f>B5+C5+D5</f>
+        <v>1340416</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>B6+C6+D6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f>B7+C7+D7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f>B8+C8+D8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>B9+C9+D9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>B10+C10+D10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>B11+C11+D11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f>B12+C12+D12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>B13+C13+D13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>B14+C14+D14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f>B15+C15+D15</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>